<commit_message>
Work Mgmt step 1
</commit_message>
<xml_diff>
--- a/doc/数据库设计.xlsx
+++ b/doc/数据库设计.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="181">
   <si>
     <t>字段描述</t>
   </si>
@@ -480,9 +480,6 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>气管内全身麻醉，腰硬联合麻醉，硬膜外麻醉，神经阻滞麻醉，支气管内麻醉，强化麻醉</t>
-  </si>
-  <si>
     <t>表名：T_ANES_WORK（麻醉工作量表）</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -495,67 +492,175 @@
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
+    <t>住院号</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>文本型数字</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>手术名称</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>麻醉方式</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>pump</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>数值型数字范围为0-1，默认为0</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>dezocine</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>数值型数字范围为0-10，默认为0</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>mepivacaine</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>手术时间</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>admission_no</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>datetime</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>tinyint</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>医生姓名</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>麻醉医生ID</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>anesthetist_id</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>T_ANESTHETIST：ID</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(3)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>性别</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>sex</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(2)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>operation_dt</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient_name</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient_age</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>operation_name</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>术后止痛泵</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>地佐辛</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>甲哌卡因</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>表名：T_ANES_ANESTHETIST（麻醉医生表）</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
     <t>department</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>普外科，妇科，产科，骨科，手足外科，脑外科，口腔科，耳鼻喉科</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>住院号</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>文本型数字</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>year</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>手术名称</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>麻醉方式</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>术后止痛泵</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>pump</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>数值型数字范围为0-1，默认为0</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>地佐辛</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>dezocine</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>数值型数字范围为0-10，默认为0</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>甲哌卡因</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>mepivacaine</t>
+    <t>varchar(2)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(2)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>anes_method</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>普外科，妇科，产科，骨科，手足外科，脑外科，口腔科，耳鼻喉科；t_sys_dict : DEPARTMENT</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>气管内全身麻醉，腰硬联合麻醉，硬膜外麻醉，神经阻滞麻醉，支气管内麻醉，强化麻醉；t_sys_dict : ANES_METHOD</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
@@ -564,82 +669,6 @@
   </si>
   <si>
     <t>病人年龄</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>手术时间</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>admission_no</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>anesthesia_method</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>datetime</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(10)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>operation</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>operation_time</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(10)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(20)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>tinyint</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>医生姓名</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>麻醉医生ID</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>anesthetist_id</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>表名：T_ANESTHETIST（麻醉医生表）</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>T_ANESTHETIST：ID</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(20)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>varchar(3)</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -1170,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H120"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
@@ -2295,7 +2324,9 @@
         <v>10</v>
       </c>
       <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
+      <c r="F64" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G64" s="4"/>
       <c r="H64" s="5" t="s">
         <v>38</v>
@@ -2444,7 +2475,9 @@
         <v>10</v>
       </c>
       <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
+      <c r="F73" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G73" s="4"/>
       <c r="H73" s="5" t="s">
         <v>38</v>
@@ -2587,7 +2620,9 @@
         <v>10</v>
       </c>
       <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
+      <c r="F82" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G82" s="4"/>
       <c r="H82" s="5" t="s">
         <v>38</v>
@@ -2655,7 +2690,7 @@
         <v>13</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -2673,7 +2708,7 @@
         <v>22</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -2774,7 +2809,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A94" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
@@ -2815,16 +2850,18 @@
         <v>8</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E96" s="4"/>
-      <c r="F96" s="4"/>
+      <c r="F96" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G96" s="4"/>
       <c r="H96" s="5" t="s">
         <v>38</v>
@@ -2832,13 +2869,13 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A97" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -2850,13 +2887,13 @@
     </row>
     <row r="98" spans="1:8" ht="33" x14ac:dyDescent="0.15">
       <c r="A98" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>137</v>
+        <v>173</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -2865,18 +2902,18 @@
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="5" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A99" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -2885,18 +2922,18 @@
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A100" s="4" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -2906,13 +2943,13 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A101" s="4" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -2922,13 +2959,13 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A102" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -2936,15 +2973,15 @@
       <c r="G102" s="4"/>
       <c r="H102" s="5"/>
     </row>
-    <row r="103" spans="1:8" ht="33" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:8" ht="49.5" x14ac:dyDescent="0.15">
       <c r="A103" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -2953,75 +2990,83 @@
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="5" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A104" s="4" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C104" s="4"/>
+        <v>155</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="F104" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="5" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A105" s="4" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C105" s="4"/>
+        <v>141</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
       <c r="H105" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A106" s="4" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C106" s="4"/>
+        <v>143</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
       <c r="H106" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A107" s="4" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C107" s="4"/>
+        <v>145</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
       <c r="H107" s="5" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.15">
@@ -3094,7 +3139,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A113" s="10" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B113" s="10"/>
       <c r="C113" s="10"/>
@@ -3135,16 +3180,18 @@
         <v>8</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D115" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E115" s="4"/>
-      <c r="F115" s="4"/>
+      <c r="F115" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G115" s="4"/>
       <c r="H115" s="5" t="s">
         <v>38</v>
@@ -3152,47 +3199,47 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A116" s="4" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
-      <c r="F116" s="4"/>
+      <c r="F116" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G116" s="4"/>
       <c r="H116" s="5"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A117" s="4" t="s">
-        <v>24</v>
+        <v>160</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>85</v>
+        <v>161</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
-      <c r="F117" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="F117" s="4"/>
       <c r="G117" s="4"/>
       <c r="H117" s="5"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:8" ht="33" x14ac:dyDescent="0.15">
       <c r="A118" s="4" t="s">
-        <v>25</v>
+        <v>163</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
@@ -3200,53 +3247,91 @@
         <v>10</v>
       </c>
       <c r="G118" s="4"/>
-      <c r="H118" s="5"/>
+      <c r="H118" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A119" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>93</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
-      <c r="F119" s="4"/>
+      <c r="F119" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G119" s="4"/>
       <c r="H119" s="5"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A120" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>27</v>
+        <v>120</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
-      <c r="F120" s="4"/>
+      <c r="F120" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G120" s="4"/>
       <c r="H120" s="5"/>
     </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A121" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D121" s="4"/>
+      <c r="E121" s="4"/>
+      <c r="F121" s="4"/>
+      <c r="G121" s="4"/>
+      <c r="H121" s="5"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A122" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D122" s="4"/>
+      <c r="E122" s="4"/>
+      <c r="F122" s="4"/>
+      <c r="G122" s="4"/>
+      <c r="H122" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A50:H50"/>
     <mergeCell ref="A113:H113"/>
     <mergeCell ref="A56:H56"/>
     <mergeCell ref="A62:H62"/>
     <mergeCell ref="A71:H71"/>
     <mergeCell ref="A80:H80"/>
     <mergeCell ref="A94:H94"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A50:H50"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>